<commit_message>
Reset to 1V8/0V8 setting
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeSupraHex-702-BOM-JLC.xlsx
+++ b/Manufacturing Files/bitaxeSupraHex-702-BOM-JLC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="150">
   <si>
     <t>Designator</t>
   </si>
@@ -338,16 +338,13 @@
     <t>R64,R38,R30</t>
   </si>
   <si>
-    <t>110k</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
     <t>SOT-23-5_HandSoldering</t>
   </si>
   <si>
-    <t>MIC5504-MS</t>
+    <t>MIC5504-1.8YM5-TR</t>
   </si>
   <si>
     <t>R4,R5</t>
@@ -395,7 +392,7 @@
     <t>R66,R32,R40</t>
   </si>
   <si>
-    <t>220k</t>
+    <t>402k</t>
   </si>
   <si>
     <t>R87,R86,R85,R84</t>
@@ -1648,8 +1645,8 @@
   <sheetPr/>
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -2107,243 +2104,243 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" t="s">
         <v>99</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>100</v>
-      </c>
-      <c r="C42" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" t="s">
         <v>106</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>107</v>
-      </c>
-      <c r="C45" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" t="s">
         <v>113</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>114</v>
-      </c>
-      <c r="C48" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" t="s">
         <v>120</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>121</v>
-      </c>
-      <c r="C51" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
         <v>123</v>
       </c>
-      <c r="B52" t="s">
-        <v>124</v>
-      </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" t="s">
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" t="s">
         <v>129</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>130</v>
-      </c>
-      <c r="C55" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B56" t="s">
         <v>23</v>
       </c>
       <c r="C56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" t="s">
         <v>134</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>135</v>
-      </c>
-      <c r="C57" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B58" t="s">
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" t="s">
         <v>139</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>140</v>
-      </c>
-      <c r="C59" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B60" t="s">
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B62">
         <v>74438357082</v>
       </c>
       <c r="C62" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B63" t="s">
         <v>25</v>
@@ -2354,10 +2351,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
-      </c>
-      <c r="B64" t="s">
-        <v>150</v>
       </c>
       <c r="C64" s="1">
         <v>824045812</v>

</xml_diff>